<commit_message>
modificari saptamana 30 29 28 27
</commit_message>
<xml_diff>
--- a/Database/Cornestean/Saptamana 27.xlsx
+++ b/Database/Cornestean/Saptamana 27.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai\Desktop\Repository Practica\Practica_covid19_UTCN\Database\Cornestean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3F366E-F061-4EE6-991B-8C5C202DF690}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31453C40-D2F6-401C-B2E8-DE485943DD68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E5ECFD75-435B-4B05-A6C2-15B3669C5D4D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E5ECFD75-435B-4B05-A6C2-15B3669C5D4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
   <si>
     <t>Total</t>
   </si>
@@ -186,6 +187,72 @@
   </si>
   <si>
     <t>Saptamana 6-12 iulie</t>
+  </si>
+  <si>
+    <t>Caracteristicile cazurilor confirmate si a deceselor</t>
+  </si>
+  <si>
+    <t>Cazuri</t>
+  </si>
+  <si>
+    <t>Varsta,mediana(range)</t>
+  </si>
+  <si>
+    <t>Sex,masculin</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>Vindecati</t>
+  </si>
+  <si>
+    <t>Personal sanitar</t>
+  </si>
+  <si>
+    <t>Afectiuni cardiovasculare</t>
+  </si>
+  <si>
+    <t>Diabet</t>
+  </si>
+  <si>
+    <t>Afectiuni neurologice</t>
+  </si>
+  <si>
+    <t>Afectiuni renale</t>
+  </si>
+  <si>
+    <t>Obezitate</t>
+  </si>
+  <si>
+    <t>Afectiuni Pulmonare</t>
+  </si>
+  <si>
+    <t>Neoplasm</t>
+  </si>
+  <si>
+    <t>Altele</t>
+  </si>
+  <si>
+    <t>Numar</t>
+  </si>
+  <si>
+    <t>Procentaj</t>
+  </si>
+  <si>
+    <t>49(0-99)</t>
+  </si>
+  <si>
+    <t>69(20-99)</t>
+  </si>
+  <si>
+    <t>94% din decese aveau comorbiditati asociate</t>
+  </si>
+  <si>
+    <t>78.4% din decese au fost la persoane de peste 60 ani</t>
+  </si>
+  <si>
+    <t>59.2% din decese au fost la barbati</t>
   </si>
 </sst>
 </file>
@@ -221,9 +288,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -544,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEA1934-77AD-4BBE-854C-7DB585E15EC2}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,23 +627,24 @@
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="34.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="47.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="4"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -594,7 +665,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -613,8 +684,11 @@
       <c r="F3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -633,8 +707,11 @@
       <c r="F4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -653,8 +730,11 @@
       <c r="F5" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -674,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -694,7 +774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -714,7 +794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -734,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -754,7 +834,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -774,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -794,7 +874,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -814,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -834,7 +914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -854,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1455,6 +1535,32 @@
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>0</v>
+      </c>
+      <c r="C46" s="3">
+        <v>32948</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1947</v>
+      </c>
+      <c r="E46" s="3">
+        <v>3725</v>
+      </c>
+      <c r="F46" s="3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1464,4 +1570,242 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6768EF5-3FB0-4EE2-AEE1-F82BE6E61EDB}">
+  <dimension ref="A1:P6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="3"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="3">
+        <v>14978</v>
+      </c>
+      <c r="D5" s="3">
+        <v>803</v>
+      </c>
+      <c r="E5" s="3">
+        <v>23552</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3422</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1125</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1256</v>
+      </c>
+      <c r="J5" s="3">
+        <v>594</v>
+      </c>
+      <c r="K5" s="3">
+        <v>428</v>
+      </c>
+      <c r="L5" s="3">
+        <v>377</v>
+      </c>
+      <c r="M5" s="3">
+        <v>330</v>
+      </c>
+      <c r="N5" s="3">
+        <v>340</v>
+      </c>
+      <c r="O5" s="3">
+        <v>230</v>
+      </c>
+      <c r="P5" s="3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3">
+        <v>45.5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="E6" s="3">
+        <v>71.5</v>
+      </c>
+      <c r="F6" s="3">
+        <v>10.4</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3">
+        <v>59.2</v>
+      </c>
+      <c r="I6" s="3">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="J6" s="3">
+        <v>31.2</v>
+      </c>
+      <c r="K6" s="3">
+        <v>22.5</v>
+      </c>
+      <c r="L6" s="3">
+        <v>19.8</v>
+      </c>
+      <c r="M6" s="3">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="N6" s="3">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="O6" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="P6" s="3">
+        <v>19.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:P3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>